<commit_message>
2 artikkelin läpikäyntiä lisätty
</commit_message>
<xml_diff>
--- a/Artikkelit.xlsx
+++ b/Artikkelit.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Artikkeli</t>
   </si>
@@ -19,9 +19,6 @@
     <t>Hyödyllisyys</t>
   </si>
   <si>
-    <t>Luettavuus</t>
-  </si>
-  <si>
     <t>Sisältö lyhyesti</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>Käy todella hyvin CA asioita läpi ja yhdistää sitä ohjelmointiin 5/5</t>
   </si>
   <si>
-    <t>Etenee hyvin ja siitä ymmärtää sanoman hyvin 4/5</t>
-  </si>
-  <si>
     <t>Käy läpi kuinka CAn eri ominaisuuksia hyödynnetään Carnegie Mellonin yliopiston yläkoululaisten robo-ohjelmointileirillä. Leirillä lapset tekivät LEGO Mindstorm roboja ja yrittivät ratkoa niiden avulla avaruusteemaisia ongelmia. Selitetään miten CA opetuksessa on toiminut heillä.</t>
   </si>
   <si>
@@ -67,9 +61,6 @@
     <t>Käy läpi kuinka tieteellistätekstiä kannattaisi kirjoittaa 2/5</t>
   </si>
   <si>
-    <t>Vaikeaa luettavaa ja ymmärrettävää - sanoma vaikeasti saatavissa 1/5</t>
-  </si>
-  <si>
     <t>Käy läpi kuinka tieteellisiä julkaisuja pitäisi tehdä, kuinka he julkaisevat tieteellisenlehtensä SciJourn (joka suunnattu nuorille). Kertoo myös kuinka he opettavat kirjoittamista eteenpäin CA:n keinoin.</t>
   </si>
   <si>
@@ -91,9 +82,6 @@
     <t>Käsittelee kuinka Carnegie Mellonin yliopistolla eri asioita pyritään opettamaan valmentamalla CA näkökulmasta 3/5</t>
   </si>
   <si>
-    <t>Melko helppoa luettavaa ja oleelliset asiat saa hyvin irti 3/5</t>
-  </si>
-  <si>
     <t>Kertoo kuinka opettaja valmentaa Carnegie Mellonin yliopistolla CAn näkökulmasta. Miten opettamisessa pitäisi hyödyntää erilaisia CAn ominaisuuksia. Ideaalisen valmentajan/opettajan ominaisuudet.</t>
   </si>
   <si>
@@ -107,6 +95,45 @@
   </si>
   <si>
     <t>E = effective, I = ineffective, N = neutral -- Kysely tehty 2009 oppilailla ja kysytty miten opetus on toiminut verrattuna muihin yliopistoihin. Techical skills: 65% E, 19% N, 16I -- Business skills: 82% E, 11% N, 7% I -- Professional skills: 88% E, 9% N, 3% I -- (116/375 henkilöstä vastasi kyselyyn) </t>
+  </si>
+  <si>
+    <t>Instructional Design of a Programming Course -- A Learning Theoretic Approach</t>
+  </si>
+  <si>
+    <t>Käsittelee ohjelmoinnin opettamista muun muossa CA:ta käyttäen Aarhusin yliopistolla 5/5</t>
+  </si>
+  <si>
+    <t>Kertoo kolmesta eri opetustekniikasta ohjelmoinnissa (cognitive load theory, CA, worked examples). Selitetään miten kutakin voi hyödyntää ohjelmoinnin opettamiseen ja kerrotaan miten Aarhusin yliopistolla näitä on hyödynnetty opetuksessa.</t>
+  </si>
+  <si>
+    <t>Käy todella hyvin erilaisia opetustekniikoita läpi ja selitetään miten niitä konkreettisesti opetuksessa ja materiaaleja suunniteltaessa voidaan hyödyntää</t>
+  </si>
+  <si>
+    <t>Guidance-fading negatiivinen vaikutus henkilöille, jotka jo omaksuneet expertisen. </t>
+  </si>
+  <si>
+    <t>400 oppilasta per vuosi, Aarhuusin yliopisto, Tanska, opetusmenetelmät olleet käytössä yli 4 vuotta kyseisessä yliopistossa</t>
+  </si>
+  <si>
+    <t>Ei ole kunnon tuloksia, mutta toiminut hyvin. Pitäisi tehdä kontrolloituja testejä tulosten muodostamiseen.</t>
+  </si>
+  <si>
+    <t>Helping Novice Programming Students Succeed</t>
+  </si>
+  <si>
+    <t>Käsittelee ohjelmoinnin opettamista käyttäen CA:ta, University of New Mexico, Valencia Campus 5/5</t>
+  </si>
+  <si>
+    <t>Kertoo aluksi pääpiirteittäin mitä on CA ja tämän jälkeen syventyy siihen, miten CA:ta voidaan hyödyntää ohjelmoinnin opettamiseen</t>
+  </si>
+  <si>
+    <t>Käy läpi oleellista asiaa, CA:n pääpiirteittäin ja miten sitä voi hyödyntää ohjelmoinnin opettamisessa</t>
+  </si>
+  <si>
+    <t>2006, University of New Mexico, Valencia Campus</t>
+  </si>
+  <si>
+    <t>Ei tuloksia, aikoivat juuri ottaa käyttöön CA:n ohjelmoinnin opetuksessa</t>
   </si>
 </sst>
 </file>
@@ -178,8 +205,8 @@
   <cols>
     <col min="1" customWidth="1" max="1" width="30.43"/>
     <col min="2" customWidth="1" max="2" width="28.29"/>
-    <col min="3" customWidth="1" max="3" width="21.71"/>
-    <col min="4" customWidth="1" max="4" width="43.29"/>
+    <col min="3" customWidth="1" max="3" width="55.14"/>
+    <col min="4" customWidth="1" max="4" width="34.43"/>
     <col min="5" customWidth="1" max="5" width="23.29"/>
     <col min="6" customWidth="1" max="6" width="32.14"/>
     <col min="7" customWidth="1" max="7" width="29.86"/>
@@ -208,86 +235,120 @@
       <c t="s" s="1" r="G4">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="H4">
-        <v>7</v>
-      </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
+        <v>7</v>
+      </c>
+      <c t="s" r="B6">
         <v>8</v>
       </c>
-      <c t="s" r="B6">
+      <c t="s" r="C6">
         <v>9</v>
       </c>
-      <c t="s" r="C6">
+      <c t="s" r="D6">
         <v>10</v>
       </c>
-      <c t="s" r="D6">
+      <c t="s" r="E6">
         <v>11</v>
       </c>
-      <c t="s" r="E6">
+      <c t="s" r="F6">
         <v>12</v>
       </c>
-      <c t="s" r="F6">
+      <c t="s" r="G6">
         <v>13</v>
-      </c>
-      <c t="s" r="G6">
-        <v>14</v>
-      </c>
-      <c t="s" r="H6">
-        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
+        <v>14</v>
+      </c>
+      <c t="s" r="B8">
+        <v>15</v>
+      </c>
+      <c t="s" r="C8">
         <v>16</v>
       </c>
-      <c t="s" r="B8">
+      <c t="s" r="D8">
         <v>17</v>
       </c>
-      <c t="s" r="C8">
+      <c t="s" r="E8">
         <v>18</v>
       </c>
-      <c t="s" r="D8">
+      <c t="s" r="F8">
         <v>19</v>
       </c>
-      <c t="s" r="E8">
+      <c t="s" r="G8">
         <v>20</v>
-      </c>
-      <c t="s" r="F8">
-        <v>21</v>
-      </c>
-      <c t="s" r="G8">
-        <v>22</v>
-      </c>
-      <c t="s" r="H8">
-        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c t="s" r="A10">
+        <v>21</v>
+      </c>
+      <c t="s" r="B10">
+        <v>22</v>
+      </c>
+      <c t="s" r="C10">
+        <v>23</v>
+      </c>
+      <c t="s" r="D10">
         <v>24</v>
       </c>
-      <c t="s" r="B10">
+      <c t="s" r="E10">
         <v>25</v>
       </c>
-      <c t="s" r="C10">
+      <c t="s" r="F10">
         <v>26</v>
       </c>
-      <c t="s" r="D10">
+      <c t="s" r="G10">
         <v>27</v>
       </c>
-      <c t="s" r="E10">
+    </row>
+    <row r="12">
+      <c t="s" r="A12">
         <v>28</v>
       </c>
-      <c t="s" r="F10">
+      <c t="s" r="B12">
         <v>29</v>
       </c>
-      <c t="s" r="G10">
+      <c t="s" r="C12">
         <v>30</v>
       </c>
-      <c t="s" r="H10">
+      <c t="s" r="D12">
         <v>31</v>
+      </c>
+      <c t="s" r="E12">
+        <v>32</v>
+      </c>
+      <c t="s" r="F12">
+        <v>33</v>
+      </c>
+      <c t="s" r="G12">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" r="A14">
+        <v>35</v>
+      </c>
+      <c t="s" r="B14">
+        <v>36</v>
+      </c>
+      <c t="s" r="C14">
+        <v>37</v>
+      </c>
+      <c t="s" r="D14">
+        <v>38</v>
+      </c>
+      <c t="s" r="E14">
+        <v>11</v>
+      </c>
+      <c t="s" r="F14">
+        <v>39</v>
+      </c>
+      <c t="s" r="G14">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Artikkelin läpikäynti lisätty jälleen
The Abstraction Transition Taxonomy: Developing Desired Learning
Outcomes through the Lens of Situated Cognition
</commit_message>
<xml_diff>
--- a/Artikkelit.xlsx
+++ b/Artikkelit.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr dateCompatibility="0"/>
+  <workbookPr/>
   <sheets>
     <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
   </sheets>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Artikkeli</t>
   </si>
@@ -58,7 +58,7 @@
     <t>A Cognitive Apprenticeship for Science Literacy Based on Journalism</t>
   </si>
   <si>
-    <t>Käy läpi kuinka tieteellistätekstiä kannattaisi kirjoittaa 2/5</t>
+    <t>Käy läpi kuinka tieteellistätekstiä kannattaisi kirjoittaa ja CA:n näkökulma asian opettamiseen 1/5</t>
   </si>
   <si>
     <t>Käy läpi kuinka tieteellisiä julkaisuja pitäisi tehdä, kuinka he julkaisevat tieteellisenlehtensä SciJourn (joka suunnattu nuorille). Kertoo myös kuinka he opettavat kirjoittamista eteenpäin CA:n keinoin.</t>
@@ -134,6 +134,45 @@
   </si>
   <si>
     <t>Ei tuloksia, aikoivat juuri ottaa käyttöön CA:n ohjelmoinnin opetuksessa</t>
+  </si>
+  <si>
+    <t>Teaching and Learning Programming and Software Engineering via Interactive Gaming</t>
+  </si>
+  <si>
+    <t>Käsittelee MOOC sivustoa Pex4Fun (pelimäinen), pari kappaletta CA:ta piilotettuna 2/5</t>
+  </si>
+  <si>
+    <t>Kerrotaan aluksi MOOC merkitys (Massive Open Online Courses). Sen jälkeen selitetään Pex4Fun sivustosta, missä voi oppia ohjelmointia. Kyseinen sivusto on pelimäinen ja samalla opettaa ohjelmointia opiskelijoille. Tehdyistä tehtävistä saa merkintöjä ylös ja voi kilpailla muitten kanssa. Duel haasteita. Pieni ripaus CA:ta miten jollakin yliopistolla professori jeesi vähän tehtävissä, jotta ei mennä liian pahasti harhaan ja masennuta.</t>
+  </si>
+  <si>
+    <t>Käydään läpi sivuston Pex4Fun melko selkeästi.</t>
+  </si>
+  <si>
+    <t>Vain muutama rivi oleellista asiaa CA:n kannalta</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Ei tuloksia</t>
+  </si>
+  <si>
+    <t>The Abstraction Transition Taxonomy: Developing Desired Learning Outcomes through the Lens of Situated Cognition</t>
+  </si>
+  <si>
+    <t>Käsittelee mitä ekspertiksi kehittyminen vaatii. CA ja deliperate practice. Käy läpi ohjelmointiin liittyviä taxonomeja ja kertoo niitten opetuksen tärkeydestä. Kertoo kuinka ohjelmointia opiskelevilla henkilöllä testailtiin clicker kysymyksiä (worked examples), joiden kuatta CA. 5/5</t>
+  </si>
+  <si>
+    <t>Kertoo mitä ekspertiksi kehittyminen vaatii CA:n/situated cognitionin pohjalta. Kertoo lyhyesti liittyviä töitä - taxonomioiden oppiminen (sanastoa opettamiseen), Apprenticeship and Deliberate Practice (Through worked examples), Acculturation (pari programming, coding dojos). Kerrotaan oppimateriaaleista yliopiston kurssilla, jossa ~570 oppilasta. Oppimateriaalit sisältivät worked exampleja (clicker questioneja), jotka pyrkivät kysymysten kautta tuomaan esiin CA:ta - WHY kysymykset tärkeitä, how kysymysten sijaan! WHY kysymykset tuovat esiin CA:n metodeja ajatteluun ja vievät ajattelua syvemmälle (expertise), työläämpiä/hankalampia arvostella. Katsottiin myös läpi yliopiston pitämiä kurssikokeiden kysymysten muodostamisia, todella vähän why kysymyksiä.</t>
+  </si>
+  <si>
+    <t>Käydään worked examples näkökulmasta CA:ta. Kuinka oikein muodostetuilla kysymyksillä WHY kysymykset HOW sijaan, luodaan paremmin ammattitaitoisuutta. Kysymystä joutuu miettimään syvemmin. Uutta näkökulmaa CA:han!</t>
+  </si>
+  <si>
+    <t>USA, yliopisto, CS Principles course (CS0-type course), ~570 oppilasta, clicker questionit (worked examples) (english, CS speak, code)</t>
+  </si>
+  <si>
+    <t>Kurssi oli onnistunut - opiskelijat kehittyivät ja näkivät teknologian mieluisampana. Abstraction Transition (AT) Taxonomy kyseisten 570 oppilaan tekemien kyselyiden perusteella (clicker questions, samalla olivat kurssimateriaaleja). Ei konkreettisia todisteita että toimiiko, mutta monet tekijät tukevat ideaa WHY kysymyksistä CA:n perusteella. </t>
   </si>
 </sst>
 </file>
@@ -351,6 +390,52 @@
         <v>40</v>
       </c>
     </row>
+    <row r="16">
+      <c t="s" r="A16">
+        <v>41</v>
+      </c>
+      <c t="s" r="B16">
+        <v>42</v>
+      </c>
+      <c t="s" r="C16">
+        <v>43</v>
+      </c>
+      <c t="s" r="D16">
+        <v>44</v>
+      </c>
+      <c t="s" r="E16">
+        <v>45</v>
+      </c>
+      <c t="s" r="F16">
+        <v>46</v>
+      </c>
+      <c t="s" r="G16">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" r="A18">
+        <v>48</v>
+      </c>
+      <c t="s" r="B18">
+        <v>49</v>
+      </c>
+      <c t="s" r="C18">
+        <v>50</v>
+      </c>
+      <c t="s" r="D18">
+        <v>51</v>
+      </c>
+      <c t="s" r="E18">
+        <v>11</v>
+      </c>
+      <c t="s" r="F18">
+        <v>52</v>
+      </c>
+      <c t="s" r="G18">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Artikkeli lisätty + aineen hahmottelu
</commit_message>
<xml_diff>
--- a/Artikkelit.xlsx
+++ b/Artikkelit.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>Artikkeli</t>
   </si>
@@ -173,6 +173,24 @@
   </si>
   <si>
     <t>Kurssi oli onnistunut - opiskelijat kehittyivät ja näkivät teknologian mieluisampana. Abstraction Transition (AT) Taxonomy kyseisten 570 oppilaan tekemien kyselyiden perusteella (clicker questions, samalla olivat kurssimateriaaleja). Ei konkreettisia todisteita että toimiiko, mutta monet tekijät tukevat ideaa WHY kysymyksistä CA:n perusteella. </t>
+  </si>
+  <si>
+    <t>The Game Studies Practicum: Applying Situated Learning to Teach Professional Practices</t>
+  </si>
+  <si>
+    <t>Käsittelee Singapore-Mit GAMBIT kesäohjelmaa, miten sitä on järjestetty ja pyritty opettamaan. Näkemystä Situated learningista ja CA:sta. 3/5</t>
+  </si>
+  <si>
+    <t>Singapore-MIT GAMBIT kesäohjelma 8 viikon mittainen ohjelmointiprojekti oppilailla (ohtuprojekti fiilis). Mutta opettamassa ohjelmointialan ammattilaisia pelientekonäkökulmasta. Ohjaavat oppilaita oikeaan suuntaan coachin. Kertoo situated learningista ja CA:sta. Selittää miten kesäohjelmaa on järjestetty ja miten siinä näkyvät nämä eri näkökulmat.</t>
+  </si>
+  <si>
+    <t>Vähän erilaista näkemystä CA:han, koska yhdistetty scrum ja ei oikein muuta CA yhteyttä. Scrumiin yhdistettyä CA ja kuinka pyritty opettamaan tätä Singapore-MIT GAMBIT kurssia. Samalla tosin epäilyttävää.</t>
+  </si>
+  <si>
+    <t>Ei tuloksia, kerrotaan vain miten kurssia on järjestetty ja vähän omituinen yhteys scrum liitteestä CA:han.</t>
+  </si>
+  <si>
+    <t>Singapore, yliopisto, (yhteistyössä MIT)</t>
   </si>
 </sst>
 </file>
@@ -436,6 +454,29 @@
         <v>53</v>
       </c>
     </row>
+    <row r="20">
+      <c t="s" r="A20">
+        <v>54</v>
+      </c>
+      <c t="s" r="B20">
+        <v>55</v>
+      </c>
+      <c t="s" r="C20">
+        <v>56</v>
+      </c>
+      <c t="s" r="D20">
+        <v>57</v>
+      </c>
+      <c t="s" r="E20">
+        <v>58</v>
+      </c>
+      <c t="s" r="F20">
+        <v>59</v>
+      </c>
+      <c t="s" r="G20">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
5 Artikkelia lisätty (pdf ja xlsx)
total nyt 10
</commit_message>
<xml_diff>
--- a/Artikkelit.xlsx
+++ b/Artikkelit.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="91">
   <si>
     <t>Artikkeli</t>
   </si>
@@ -191,6 +191,99 @@
   </si>
   <si>
     <t>Singapore, yliopisto, (yhteistyössä MIT)</t>
+  </si>
+  <si>
+    <t>Extreme Apprenticeship Method: Key Practices and Upward Scalability</t>
+  </si>
+  <si>
+    <t>Käsittelee XA:ta ohjelmoinnin opetuksessa. Kertoo miten Helsingin yliopistolla järjestetty ohjelmointikursseja XA:ta käyttäen. Pajaohjausta/Scaffolding. 5/5</t>
+  </si>
+  <si>
+    <t>Pajaohjelmointia ollut useammalla kurssilla käytössä. Paljon tehtäviä. Kertoo kuinka järjestetty, paljonko ohjaajia ja oppilaita. Sisältää tuloksia. Kertoo tosi hyvin scaffolding näkökulmaa pajaohjauksessa ja ripauksen tehtävien suhteen.</t>
+  </si>
+  <si>
+    <t>Scaffolding pajaohjaus/tehtävät. Tuloksia!</t>
+  </si>
+  <si>
+    <t>Helsingin yliopisto, n =192 and 147, 2010, ohjelmoinnin perus- ja jatkokurssit</t>
+  </si>
+  <si>
+    <t>Kurssin läpäisy prosentti kasvoi keskiarvoon verrattuna ~25%.</t>
+  </si>
+  <si>
+    <t>Scaffolding Students' Learning using Test My Code</t>
+  </si>
+  <si>
+    <t>Käsittelee Helsingin yliopiston monilla ohjelmointikursseilla käytössä olevaa Test My Code (TMC). Paljon tehtäviä/palaute/scaffolding. 5/5</t>
+  </si>
+  <si>
+    <t>Helsingin yliopistolla ohjelmointikursseilla käytössä ollut TMC. Kerrotaan kuinka TMC:ta sovelletaan ja kuinka se soveltuu scaffolding näkökulmassa, voi antaa palautetta, paljon tehtäviä ja opettaa testausta. Vie vähemmän aikaa ohjaajilta, koska tehtäviä ei tarvitse tarkistaa. Opiskelijat saavat heti palautetta tehtävää tekiessä/testit.</t>
+  </si>
+  <si>
+    <t>TMC, selitetään scaffoldingia hyvin tehtävien/palautteen kautta.</t>
+  </si>
+  <si>
+    <t>Helsingin yliopisto</t>
+  </si>
+  <si>
+    <t>Ei sinäänsä tuloksia, todetaan et toiminut hyvin.</t>
+  </si>
+  <si>
+    <t>Elementary Students' Perceptions of Social Networks: Development, Experience, and Equity in Collaborative Software Design Activities</t>
+  </si>
+  <si>
+    <t>Kai jonkin näköistä "paremmalta" katsomista ja oppimista, ihan järkyttävän epämääräistä tosin 1/5. Ei oikeastaan -mitään- hyödynnettävää.</t>
+  </si>
+  <si>
+    <t>&lt;-----</t>
+  </si>
+  <si>
+    <t>pskaa -_-</t>
+  </si>
+  <si>
+    <t>Liikaa mutustelua, vähän tietoa :lllll Kannattaako näitä proceedingei ees lukea?</t>
+  </si>
+  <si>
+    <t>Haastateltiin 131  4-5 luokkalaista lasta. 10 viikon mittaisia projekteja.</t>
+  </si>
+  <si>
+    <t>Jotain mutustelua, kuinka "old-timerit" auttoivat uusia neuvomalla heitä. Hyvän oppimisympäristön luominen ei ole pelkästään taitotasojen yhtenäisyyksistä kiinni, vaan voi olla eritasoisia oppilaita</t>
+  </si>
+  <si>
+    <t>Learning Agile Software Engineering Practices using Coding Dojo</t>
+  </si>
+  <si>
+    <t>Pair programming ja TDD. Scaffoldingia. CA:ta vähän suoraan ja paljon epäsuorasti, voi olla kuitenki hyödyllistä! 4/5</t>
+  </si>
+  <si>
+    <t>Kertoo coding dojoista, kuinka niissä voi tehokkaasti oppia Agilen menetelmiä (pariohjelmointia/ryhmässä tehtävän tekoa/ test-driven.development). Kertoo erityyppisistä dojoista ja mitä niissä tehdään. Cognitive apprenticeshippiä epäsuorasti, voi olla oleellista asiaa! Kertoo kuinka ohtu-kurssilla testattu erästä varianttia.</t>
+  </si>
+  <si>
+    <t>Coding dojo, analyysia, CA:ta paljon epäsuorasti (eli ei analysoitu CA:n kannalta suoraan)!</t>
+  </si>
+  <si>
+    <t>73 oppilasta, 15 sessiota, Helsingin yliopisto, Ohtu-kurssi</t>
+  </si>
+  <si>
+    <t>Kyselyn perusteella dojo ei ollut kilailuhenkinen ja ilmapiiri oli rento. Oppilaiden mielestä hyvän ohjelmoinnin hyödyllisyys tuli näkyviin dojossa ja se soveltuu ohjelmointi taitojen kehittämiseen. Melkein puolet oppilaista sai "Ahaa" elämyksiä. 80% oppilaista suosittelisi dojoa muillekkin, 70% osallistuisi dojoihin jatkossakin. Oppilaat kokivat ymmärtäneensä TDD ja pariohjelmoinnin tavoitteet ja oppivat varomaan ylisuunnittelemaan/rakentamaan ratkaisun.</t>
+  </si>
+  <si>
+    <t>Multi-faceted Support for MOOC in Programming</t>
+  </si>
+  <si>
+    <t>XA:ta, Scaffoldingia 4/5</t>
+  </si>
+  <si>
+    <t>Kertoo Helsingin yliopiston MOOC:ista, 3 tärkeää pointtia siinä XA, Scaffolding ja kannustaa sitoutumista kurssiin (parempi ku muut vastaavat ohjelmointikurssit). Miten toiminut, mitä siihen kuuluu (TMC), tehtävien rakenne. Kannustava. Tehtäviä PALJON (Scaffolding).</t>
+  </si>
+  <si>
+    <t>Scaffolding, dataa oppilaitten palautteista (tehtävä kohtaisista)</t>
+  </si>
+  <si>
+    <t>MOOC, Helsingin yliopisto, Etäkurssi (etä palaute)</t>
+  </si>
+  <si>
+    <t>Dataa 7. luvussa paljonko osallistujia/läpäisy prosentti/kuinka moni halusi opiskelemaan. Tehtävien vaikeus/hyödyllisyys kurvi.</t>
   </si>
 </sst>
 </file>
@@ -266,7 +359,7 @@
     <col min="4" customWidth="1" max="4" width="34.43"/>
     <col min="5" customWidth="1" max="5" width="23.29"/>
     <col min="6" customWidth="1" max="6" width="32.14"/>
-    <col min="7" customWidth="1" max="7" width="29.86"/>
+    <col min="7" customWidth="1" max="7" width="47.29"/>
     <col min="8" customWidth="1" max="8" width="35.29"/>
   </cols>
   <sheetData>
@@ -477,6 +570,118 @@
         <v>47</v>
       </c>
     </row>
+    <row r="22">
+      <c t="s" r="A22">
+        <v>60</v>
+      </c>
+      <c t="s" r="B22">
+        <v>61</v>
+      </c>
+      <c t="s" r="C22">
+        <v>62</v>
+      </c>
+      <c t="s" r="D22">
+        <v>63</v>
+      </c>
+      <c t="s" r="E22">
+        <v>11</v>
+      </c>
+      <c t="s" r="F22">
+        <v>64</v>
+      </c>
+      <c t="s" r="G22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" r="A24">
+        <v>66</v>
+      </c>
+      <c t="s" r="B24">
+        <v>67</v>
+      </c>
+      <c t="s" r="C24">
+        <v>68</v>
+      </c>
+      <c t="s" r="D24">
+        <v>69</v>
+      </c>
+      <c t="s" r="F24">
+        <v>70</v>
+      </c>
+      <c t="s" r="G24">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" r="A26">
+        <v>72</v>
+      </c>
+      <c t="s" r="B26">
+        <v>73</v>
+      </c>
+      <c t="s" r="C26">
+        <v>74</v>
+      </c>
+      <c t="s" r="D26">
+        <v>75</v>
+      </c>
+      <c t="s" r="E26">
+        <v>76</v>
+      </c>
+      <c t="s" r="F26">
+        <v>77</v>
+      </c>
+      <c t="s" r="G26">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28">
+      <c t="s" r="A28">
+        <v>79</v>
+      </c>
+      <c t="s" r="B28">
+        <v>80</v>
+      </c>
+      <c t="s" r="C28">
+        <v>81</v>
+      </c>
+      <c t="s" r="D28">
+        <v>82</v>
+      </c>
+      <c t="s" r="E28">
+        <v>11</v>
+      </c>
+      <c t="s" r="F28">
+        <v>83</v>
+      </c>
+      <c t="s" r="G28">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30">
+      <c t="s" r="A30">
+        <v>85</v>
+      </c>
+      <c t="s" r="B30">
+        <v>86</v>
+      </c>
+      <c t="s" r="C30">
+        <v>87</v>
+      </c>
+      <c t="s" r="D30">
+        <v>88</v>
+      </c>
+      <c t="s" r="E30">
+        <v>11</v>
+      </c>
+      <c t="s" r="F30">
+        <v>89</v>
+      </c>
+      <c t="s" r="G30">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>